<commit_message>
✨ feat: Add K Means training results
</commit_message>
<xml_diff>
--- a/tarea1/doc/Tarea1.xlsx
+++ b/tarea1/doc/Tarea1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Universidad\Semestre 9\Estadistica III\Statistics_III\tarea1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD2BA08-3AD1-4E1E-89E5-8115EC05C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83CA432-77A2-4E6A-BB1C-F13CCD7E4C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,14 @@
     <sheet name="Punto 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Datos!$C$4:$C$33</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Datos!$D$4:$D$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Datos!$E$4:$E$33</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Datos!$G$4:$G$33</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Datos!$F$4:$F$33</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Datos!$G$4:$G$33</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Datos!$H$4:$H$33</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Datos!$E$4:$E$33</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Datos!$B$4:$B$33</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Datos!$H$4:$H$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Datos!$F$4:$F$33</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Datos!$C$4:$C$33</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Datos!$D$4:$D$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Datos!$E$4:$E$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
   <si>
     <t>City</t>
   </si>
@@ -329,6 +330,54 @@
     <t>Teniendo en cuenta los resultados de los datos de PIB y población utilizando las métricas de covarianza y correlación, se observa una relación muy estrecha entre ambas variables. Estos resultados tan positivos de ambas métricas indican que el comportamiento del PIB y la población está fuertemente relacionado, lo que podría sugerir que factores demográficos juegan un papel crucial en el crecimiento económico. Esta relación nos permite inferir que los países o regiones con mayores poblaciones tienden a generar una mayor actividad económica, reflejada en el aumento del PIB según este conjunto de datos.
 Este resultado refuerza el concepto de que la correlación es una versión estandarizada de la covarianza, lo que permite comparar más fácilmente diferentes pares de variables. Mientras que la covarianza mide cómo dos variables cambian juntas, la correlación estandariza este cambio, facilitando el análisis de las relaciones entre diferentes conjuntos de datos.</t>
   </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Mocoa (test)</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Aplicación K Means con datos de entrenamiento</t>
+  </si>
+  <si>
+    <t>dis_C1</t>
+  </si>
+  <si>
+    <t>dis_C2</t>
+  </si>
+  <si>
+    <t>dis_C3</t>
+  </si>
+  <si>
+    <t>dis_C4</t>
+  </si>
+  <si>
+    <t>dis_C5</t>
+  </si>
+  <si>
+    <t>dis_C0</t>
+  </si>
+  <si>
+    <t>Ejemplo de la primera iteración que se ve a detalle en la carpeta SRC</t>
+  </si>
+  <si>
+    <t>GDP (USD Billion)</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>San Andrés</t>
+  </si>
+  <si>
+    <t>Santa Marta</t>
+  </si>
+  <si>
+    <t>Centroides Iteración 0</t>
+  </si>
 </sst>
 </file>
 
@@ -336,10 +385,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,8 +445,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +462,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1053,60 +1114,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1141,21 +1148,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1175,35 +1167,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1214,48 +1182,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1266,9 +1192,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1292,8 +1215,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,6 +1259,78 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1338,6 +1366,106 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1424,7 +1552,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1489,7 +1617,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1554,7 +1682,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1619,7 +1747,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1684,7 +1812,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1749,7 +1877,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5705,7 +5833,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>369617</xdr:colOff>
+      <xdr:colOff>164989</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>138547</xdr:rowOff>
     </xdr:to>
@@ -5742,16 +5870,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>158290</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>188769</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>574035</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>69499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>624504</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>67912</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>83127</xdr:rowOff>
+      <xdr:rowOff>13253</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5774,8 +5902,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15342872" y="2322369"/>
-          <a:ext cx="4414759" cy="3510394"/>
+          <a:off x="15277322" y="2421760"/>
+          <a:ext cx="4264660" cy="3435702"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5786,16 +5914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>642851</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>149627</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>576590</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>36983</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>642708</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>27710</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>576447</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>107223</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5818,8 +5946,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22934815" y="2283227"/>
-          <a:ext cx="4738110" cy="3494119"/>
+          <a:off x="22436051" y="2574774"/>
+          <a:ext cx="4770639" cy="3562188"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5830,16 +5958,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>16625</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>105296</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>573216</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>32409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>376131</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>137593</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>79513</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5862,8 +5990,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="31785098" y="2432860"/>
-          <a:ext cx="4308051" cy="3289067"/>
+          <a:off x="31179112" y="2755731"/>
+          <a:ext cx="4335158" cy="3353521"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5874,16 +6002,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>692729</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>124691</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>281912</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>1256</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>385569</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>33132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5906,8 +6034,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="39568584" y="2452255"/>
-          <a:ext cx="4046780" cy="2937164"/>
+          <a:off x="38839112" y="3066674"/>
+          <a:ext cx="4079309" cy="2996197"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5918,15 +6046,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>58</xdr:col>
-      <xdr:colOff>483128</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>728293</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>130827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>312008</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>557173</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>10884</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5950,8 +6078,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="47520299" y="2286198"/>
-          <a:ext cx="3802166" cy="3189315"/>
+          <a:off x="46441667" y="3039679"/>
+          <a:ext cx="3804532" cy="3193101"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5962,16 +6090,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>67</xdr:col>
-      <xdr:colOff>117763</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>122912</xdr:rowOff>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>303293</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>71</xdr:col>
-      <xdr:colOff>185057</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>76202</xdr:rowOff>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>370587</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>102706</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5994,8 +6122,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54306849" y="2474226"/>
-          <a:ext cx="3245922" cy="2881547"/>
+          <a:off x="53172841" y="3243799"/>
+          <a:ext cx="3247816" cy="2888646"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6013,7 +6141,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>421159</xdr:colOff>
+      <xdr:colOff>45420</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>71370</xdr:rowOff>
     </xdr:to>
@@ -6056,8 +6184,8 @@
       <xdr:rowOff>47377</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>321557</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>734712</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>32136</xdr:rowOff>
     </xdr:to>
@@ -6094,16 +6222,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>598804</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>78442</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>380143</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>74897</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>163129</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>445958</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>4103</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6139,8 +6267,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12624549" y="1242224"/>
-              <a:ext cx="2634930" cy="5487960"/>
+              <a:off x="12492630" y="1463294"/>
+              <a:ext cx="2656615" cy="5564461"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6172,16 +6300,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>143742</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>162792</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>471402</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>129887</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>478028</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>30495</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6217,8 +6345,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="20066578" y="1132610"/>
-              <a:ext cx="2696788" cy="5744441"/>
+              <a:off x="19624437" y="1229592"/>
+              <a:ext cx="2713052" cy="6010086"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6250,16 +6378,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>116033</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>738886</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>79663</xdr:rowOff>
+      <xdr:rowOff>165802</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>637309</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>465031</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>27709</xdr:rowOff>
+      <xdr:rowOff>113848</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6295,8 +6423,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="27935960" y="2213263"/>
-              <a:ext cx="3680113" cy="3744191"/>
+              <a:off x="27369129" y="2325906"/>
+              <a:ext cx="3701798" cy="3817681"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6328,15 +6456,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>484910</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>304799</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>233119</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>159025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>484909</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>233118</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>83127</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6373,8 +6501,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="36201928" y="1925781"/>
-              <a:ext cx="3158836" cy="3906982"/>
+              <a:off x="35609797" y="2319129"/>
+              <a:ext cx="3180521" cy="3985894"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6406,16 +6534,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>193963</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>110836</xdr:rowOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>472259</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>24696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
-      <xdr:colOff>374073</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>652369</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6451,8 +6579,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="43808072" y="2064327"/>
-              <a:ext cx="3338946" cy="3477491"/>
+              <a:off x="43005111" y="2748018"/>
+              <a:ext cx="3360632" cy="3540138"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6484,16 +6612,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>424543</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>656456</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>65787</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>67</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>308113</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6529,8 +6657,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="51435000" y="2188028"/>
-              <a:ext cx="2830286" cy="3429001"/>
+              <a:off x="50345482" y="2789109"/>
+              <a:ext cx="2832179" cy="3432787"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6562,16 +6690,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>71</xdr:col>
-      <xdr:colOff>239486</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>130628</xdr:rowOff>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>444895</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>526868</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>732277</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>174408</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6607,8 +6735,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="57607200" y="1502228"/>
-              <a:ext cx="2671354" cy="4044044"/>
+              <a:off x="56494965" y="2350367"/>
+              <a:ext cx="2672773" cy="4045937"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6906,8 +7034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6917,40 +7045,40 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="80" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="36"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="81"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -7657,7 +7785,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B31" s="1">
         <v>0.8</v>
@@ -7735,14 +7863,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7751,10 +7879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFCB991-11F5-476A-BBAB-A17BAC111175}">
-  <dimension ref="A2:S72"/>
+  <dimension ref="A2:S125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P74" sqref="P74"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7764,8 +7892,12 @@
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
     <col min="13" max="13" width="17.77734375" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7803,31 +7935,31 @@
       <c r="A4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="41">
         <f>AVERAGE(Datos!B4:B33)</f>
         <v>8.7500000000000018</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="35">
         <f>AVERAGE(Datos!C4:C33)</f>
         <v>0.73099999999999987</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="35">
         <f>AVERAGE(Datos!D4:D33)</f>
         <v>13.833333333333334</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="35">
         <f>AVERAGE(Datos!E4:E33)</f>
         <v>29.233333333333334</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="35">
         <f>AVERAGE(Datos!F4:F33)</f>
         <v>51.5</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="35">
         <f>AVERAGE(Datos!G4:G33)</f>
         <v>48.5</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="36">
         <f>AVERAGE(Datos!H4:H33)</f>
         <v>1.6499999999999997</v>
       </c>
@@ -7836,31 +7968,31 @@
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="37">
         <f>MEDIAN(Datos!B4:B33)</f>
         <v>2.65</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="37">
         <f>MEDIAN(Datos!C4:C33)</f>
         <v>0.39</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="37">
         <f>MEDIAN(Datos!D4:D33)</f>
         <v>13.45</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="37">
         <f>MEDIAN(Datos!E4:E33)</f>
         <v>29</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="37">
         <f>MEDIAN(Datos!F4:F33)</f>
         <v>51</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="37">
         <f>MEDIAN(Datos!G4:G33)</f>
         <v>49</v>
       </c>
-      <c r="H5" s="56">
+      <c r="H5" s="38">
         <f>MEDIAN(Datos!H4:H33)</f>
         <v>0.6</v>
       </c>
@@ -7881,113 +8013,113 @@
         <f>_xlfn.STDEV.P(Datos!D4:D33)</f>
         <v>2.8955521446215071</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="37">
         <f>_xlfn.STDEV.P(Datos!E4:E33)</f>
         <v>2.2012622641465405</v>
       </c>
-      <c r="F6" s="55">
+      <c r="F6" s="37">
         <f>_xlfn.STDEV.P(Datos!F4:F33)</f>
         <v>0.76376261582597338</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="37">
         <f>_xlfn.STDEV.P(Datos!G4:G33)</f>
         <v>0.76376261582597338</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="38">
         <f>_xlfn.STDEV.P(Datos!H4:H33)</f>
         <v>3.393179433314228</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="46" t="str" cm="1">
+      <c r="B7" s="95" t="str" cm="1">
         <f t="array" ref="B7">IFERROR(_xlfn.MODE.MULT(Datos!B4:B33),"La variable no tiene Moda")</f>
         <v>La variable no tiene Moda</v>
       </c>
-      <c r="C7" s="55" cm="1">
+      <c r="C7" s="37" cm="1">
         <f t="array" ref="C7:C8">_xlfn.MODE.MULT(Datos!C4:C33)</f>
         <v>0.08</v>
       </c>
-      <c r="D7" s="46" t="str" cm="1">
+      <c r="D7" s="95" t="str" cm="1">
         <f t="array" ref="D7">IFERROR(_xlfn.MODE.MULT(Datos!D4:D33),"La variable no tiene Moda")</f>
         <v>La variable no tiene Moda</v>
       </c>
-      <c r="E7" s="47" cm="1">
+      <c r="E7" s="96" cm="1">
         <f t="array" ref="E7">_xlfn.MODE.MULT(Datos!E4:E33)</f>
         <v>29</v>
       </c>
-      <c r="F7" s="47" cm="1">
+      <c r="F7" s="96" cm="1">
         <f t="array" ref="F7">_xlfn.MODE.MULT(Datos!F4:F33)</f>
         <v>51</v>
       </c>
-      <c r="G7" s="47" cm="1">
+      <c r="G7" s="96" cm="1">
         <f t="array" ref="G7">_xlfn.MODE.MULT(Datos!G4:G33)</f>
         <v>49</v>
       </c>
-      <c r="H7" s="56" cm="1">
+      <c r="H7" s="38" cm="1">
         <f t="array" ref="H7:H8">_xlfn.MODE.MULT(Datos!H4:H33)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="55">
+      <c r="A8" s="94"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="37">
         <v>0.01</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="56">
+      <c r="D8" s="95"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="38">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="60">
+      <c r="C9" s="42">
         <f>COUNTIF(Datos!C4:C33,'Punto 1'!C7)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="101">
         <f>COUNTIF(Datos!E4:E33,'Punto 1'!E7)</f>
         <v>6</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="101">
         <f>COUNTIF(Datos!F4:F33,'Punto 1'!F7)</f>
         <v>14</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="101">
         <f>COUNTIF(Datos!G4:G33,'Punto 1'!G7)</f>
         <v>14</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="39">
         <f>COUNTIF(Datos!H4:H33,'Punto 1'!H7)</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="61">
+      <c r="A10" s="98"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="43">
         <f>COUNTIF(Datos!C4:C33,'Punto 1'!C8)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="58">
+      <c r="D10" s="100"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="40">
         <f>COUNTIF(Datos!H4:H33,'Punto 1'!H8)</f>
         <v>3</v>
       </c>
@@ -8044,11 +8176,11 @@
         <f>MIN(Datos!E4:E339)</f>
         <v>24</v>
       </c>
-      <c r="F16" s="109">
+      <c r="F16" s="64">
         <f>MIN(Datos!F4:F339)</f>
         <v>50</v>
       </c>
-      <c r="G16" s="109">
+      <c r="G16" s="64">
         <f>MIN(Datos!G4:G339)</f>
         <v>47</v>
       </c>
@@ -8077,11 +8209,11 @@
         <f>_xlfn.QUARTILE.EXC(Datos!E4:E33,1)</f>
         <v>28</v>
       </c>
-      <c r="F17" s="110">
+      <c r="F17" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!F4:F33,1)</f>
         <v>51</v>
       </c>
-      <c r="G17" s="110">
+      <c r="G17" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!G4:G33,1)</f>
         <v>48</v>
       </c>
@@ -8110,11 +8242,11 @@
         <f>_xlfn.QUARTILE.EXC(Datos!E4:E33,2)</f>
         <v>29</v>
       </c>
-      <c r="F18" s="110">
+      <c r="F18" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!F4:F33,2)</f>
         <v>51</v>
       </c>
-      <c r="G18" s="110">
+      <c r="G18" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!G4:G33,2)</f>
         <v>49</v>
       </c>
@@ -8143,11 +8275,11 @@
         <f>_xlfn.QUARTILE.EXC(Datos!E4:E33,3)</f>
         <v>31</v>
       </c>
-      <c r="F19" s="110">
+      <c r="F19" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!F4:F33,3)</f>
         <v>52</v>
       </c>
-      <c r="G19" s="110">
+      <c r="G19" s="65">
         <f>_xlfn.QUARTILE.EXC(Datos!G4:G33,3)</f>
         <v>49</v>
       </c>
@@ -8176,11 +8308,11 @@
         <f>MAX(Datos!E4:E33)</f>
         <v>33</v>
       </c>
-      <c r="F20" s="110">
+      <c r="F20" s="65">
         <f>MAX(Datos!F4:F33)</f>
         <v>53</v>
       </c>
-      <c r="G20" s="110">
+      <c r="G20" s="65">
         <f>MAX(Datos!G4:G33)</f>
         <v>50</v>
       </c>
@@ -8209,11 +8341,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F21" s="110">
+      <c r="F21" s="65">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G21" s="110">
+      <c r="G21" s="65">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -8242,11 +8374,11 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="F22" s="111">
+      <c r="F22" s="66">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="G22" s="111">
+      <c r="G22" s="66">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -8257,116 +8389,116 @@
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="90"/>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="49"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="90"/>
     </row>
     <row r="32" spans="1:8" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="126" t="s">
+      <c r="B32" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="128"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="93"/>
     </row>
     <row r="40" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="34" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B41" s="64" t="s">
+      <c r="B41" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="75" t="s">
+      <c r="E41" s="107" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="76" t="s">
+      <c r="G41" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="H41" s="77"/>
-      <c r="I41" s="75" t="s">
+      <c r="H41" s="111"/>
+      <c r="I41" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="J41" s="106" t="s">
+      <c r="J41" s="130" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" spans="2:19" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="66"/>
-      <c r="C42" s="67"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86"/>
-      <c r="H42" s="87"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="107"/>
-      <c r="L42" s="108"/>
-      <c r="M42" s="108"/>
-      <c r="N42" s="108"/>
-      <c r="O42" s="108"/>
-      <c r="P42" s="108"/>
-      <c r="Q42" s="108"/>
-      <c r="R42" s="108"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="106"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="110"/>
+      <c r="G42" s="110"/>
+      <c r="H42" s="112"/>
+      <c r="I42" s="108"/>
+      <c r="J42" s="131"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
     </row>
     <row r="43" spans="2:19" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="68">
+      <c r="B43" s="45">
         <v>103.5</v>
       </c>
-      <c r="C43" s="69">
+      <c r="C43" s="46">
         <v>7.18</v>
       </c>
-      <c r="E43" s="82">
+      <c r="E43" s="55">
         <f>B43-$B$4</f>
         <v>94.75</v>
       </c>
-      <c r="F43" s="83">
+      <c r="F43" s="56">
         <f>C43-$C$4</f>
         <v>6.4489999999999998</v>
       </c>
-      <c r="G43" s="84">
+      <c r="G43" s="86">
         <f>E43*F43</f>
         <v>611.04274999999996</v>
       </c>
-      <c r="H43" s="103"/>
+      <c r="H43" s="87"/>
       <c r="I43" s="27">
         <f>POWER(E43,2)</f>
         <v>8977.5625</v>
@@ -8375,42 +8507,42 @@
         <f>POWER(F43,2)</f>
         <v>41.589600999999995</v>
       </c>
-      <c r="L43" s="92" t="s">
+      <c r="L43" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="M43" s="89">
+      <c r="M43" s="58">
         <f>SUM(G43:H72)</f>
         <v>773.87149999999986</v>
       </c>
-      <c r="N43" s="94" t="s">
+      <c r="N43" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="O43" s="95"/>
-      <c r="P43" s="95"/>
-      <c r="Q43" s="95"/>
-      <c r="R43" s="95"/>
-      <c r="S43" s="96"/>
+      <c r="O43" s="133"/>
+      <c r="P43" s="133"/>
+      <c r="Q43" s="133"/>
+      <c r="R43" s="133"/>
+      <c r="S43" s="134"/>
     </row>
     <row r="44" spans="2:19" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="68">
+      <c r="B44" s="45">
         <v>44.1</v>
       </c>
-      <c r="C44" s="69">
+      <c r="C44" s="46">
         <v>2.57</v>
       </c>
-      <c r="E44" s="78">
+      <c r="E44" s="52">
         <f t="shared" ref="E44:E72" si="2">B44-$B$4</f>
         <v>35.35</v>
       </c>
-      <c r="F44" s="74">
+      <c r="F44" s="51">
         <f t="shared" ref="F44:F72" si="3">C44-$C$4</f>
         <v>1.839</v>
       </c>
-      <c r="G44" s="63">
+      <c r="G44" s="113">
         <f t="shared" ref="G44:G72" si="4">E44*F44</f>
         <v>65.008650000000003</v>
       </c>
-      <c r="H44" s="104"/>
+      <c r="H44" s="114"/>
       <c r="I44" s="27">
         <f>POWER(E44,2)</f>
         <v>1249.6225000000002</v>
@@ -8422,37 +8554,37 @@
       <c r="L44" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="M44" s="90">
+      <c r="M44" s="59">
         <f>COUNT(B43:B72)</f>
         <v>30</v>
       </c>
-      <c r="N44" s="97"/>
-      <c r="O44" s="98"/>
-      <c r="P44" s="98"/>
-      <c r="Q44" s="98"/>
-      <c r="R44" s="98"/>
-      <c r="S44" s="99"/>
+      <c r="N44" s="135"/>
+      <c r="O44" s="136"/>
+      <c r="P44" s="136"/>
+      <c r="Q44" s="136"/>
+      <c r="R44" s="136"/>
+      <c r="S44" s="137"/>
     </row>
     <row r="45" spans="2:19" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="68">
+      <c r="B45" s="45">
         <v>22.4</v>
       </c>
-      <c r="C45" s="69">
+      <c r="C45" s="46">
         <v>2.23</v>
       </c>
-      <c r="E45" s="78">
+      <c r="E45" s="52">
         <f>B45-$B$4</f>
         <v>13.649999999999997</v>
       </c>
-      <c r="F45" s="74">
+      <c r="F45" s="51">
         <f t="shared" si="3"/>
         <v>1.4990000000000001</v>
       </c>
-      <c r="G45" s="63">
+      <c r="G45" s="113">
         <f t="shared" si="4"/>
         <v>20.461349999999996</v>
       </c>
-      <c r="H45" s="104"/>
+      <c r="H45" s="114"/>
       <c r="I45" s="27">
         <f>POWER(E45,2)</f>
         <v>186.32249999999991</v>
@@ -8461,40 +8593,40 @@
         <f t="shared" si="5"/>
         <v>2.2470010000000005</v>
       </c>
-      <c r="L45" s="93" t="s">
+      <c r="L45" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="M45" s="91">
+      <c r="M45" s="60">
         <f>M43/M44</f>
         <v>25.79571666666666</v>
       </c>
-      <c r="N45" s="100"/>
-      <c r="O45" s="101"/>
-      <c r="P45" s="101"/>
-      <c r="Q45" s="101"/>
-      <c r="R45" s="101"/>
-      <c r="S45" s="102"/>
+      <c r="N45" s="138"/>
+      <c r="O45" s="139"/>
+      <c r="P45" s="139"/>
+      <c r="Q45" s="139"/>
+      <c r="R45" s="139"/>
+      <c r="S45" s="140"/>
     </row>
     <row r="46" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="68">
+      <c r="B46" s="45">
         <v>16.8</v>
       </c>
-      <c r="C46" s="69">
+      <c r="C46" s="46">
         <v>1.23</v>
       </c>
-      <c r="E46" s="78">
+      <c r="E46" s="52">
         <f t="shared" si="2"/>
         <v>8.0499999999999989</v>
       </c>
-      <c r="F46" s="74">
+      <c r="F46" s="51">
         <f t="shared" si="3"/>
         <v>0.49900000000000011</v>
       </c>
-      <c r="G46" s="63">
+      <c r="G46" s="113">
         <f t="shared" si="4"/>
         <v>4.0169500000000005</v>
       </c>
-      <c r="H46" s="104"/>
+      <c r="H46" s="114"/>
       <c r="I46" s="27">
         <f t="shared" ref="I46:I72" si="6">POWER(E46,2)</f>
         <v>64.802499999999981</v>
@@ -8503,32 +8635,32 @@
         <f t="shared" si="5"/>
         <v>0.24900100000000011</v>
       </c>
-      <c r="L46" s="62"/>
-      <c r="M46" s="62"/>
-      <c r="N46" s="62"/>
-      <c r="O46" s="62"/>
-      <c r="P46" s="62"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="44"/>
     </row>
     <row r="47" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="68">
+      <c r="B47" s="45">
         <v>10.5</v>
       </c>
-      <c r="C47" s="69">
+      <c r="C47" s="46">
         <v>1.03</v>
       </c>
-      <c r="E47" s="78">
+      <c r="E47" s="52">
         <f t="shared" si="2"/>
         <v>1.7499999999999982</v>
       </c>
-      <c r="F47" s="74">
+      <c r="F47" s="51">
         <f t="shared" si="3"/>
         <v>0.29900000000000015</v>
       </c>
-      <c r="G47" s="63">
+      <c r="G47" s="113">
         <f t="shared" si="4"/>
         <v>0.52324999999999977</v>
       </c>
-      <c r="H47" s="104"/>
+      <c r="H47" s="114"/>
       <c r="I47" s="27">
         <f t="shared" si="6"/>
         <v>3.0624999999999938</v>
@@ -8539,25 +8671,25 @@
       </c>
     </row>
     <row r="48" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="68">
+      <c r="B48" s="45">
         <v>7.3</v>
       </c>
-      <c r="C48" s="69">
+      <c r="C48" s="46">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E48" s="78">
+      <c r="E48" s="52">
         <f t="shared" si="2"/>
         <v>-1.450000000000002</v>
       </c>
-      <c r="F48" s="74">
+      <c r="F48" s="51">
         <f t="shared" si="3"/>
         <v>-0.15099999999999991</v>
       </c>
-      <c r="G48" s="63">
+      <c r="G48" s="113">
         <f t="shared" si="4"/>
         <v>0.21895000000000017</v>
       </c>
-      <c r="H48" s="104"/>
+      <c r="H48" s="114"/>
       <c r="I48" s="27">
         <f t="shared" si="6"/>
         <v>2.1025000000000058</v>
@@ -8568,25 +8700,25 @@
       </c>
     </row>
     <row r="49" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="68">
+      <c r="B49" s="45">
         <v>6.2</v>
       </c>
-      <c r="C49" s="69">
+      <c r="C49" s="46">
         <v>0.48</v>
       </c>
-      <c r="E49" s="78">
+      <c r="E49" s="52">
         <f t="shared" si="2"/>
         <v>-2.5500000000000016</v>
       </c>
-      <c r="F49" s="74">
+      <c r="F49" s="51">
         <f t="shared" si="3"/>
         <v>-0.25099999999999989</v>
       </c>
-      <c r="G49" s="63">
+      <c r="G49" s="113">
         <f t="shared" si="4"/>
         <v>0.64005000000000012</v>
       </c>
-      <c r="H49" s="104"/>
+      <c r="H49" s="114"/>
       <c r="I49" s="27">
         <f t="shared" si="6"/>
         <v>6.5025000000000084</v>
@@ -8597,25 +8729,25 @@
       </c>
     </row>
     <row r="50" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="68">
+      <c r="B50" s="45">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C50" s="69">
+      <c r="C50" s="46">
         <v>0.76</v>
       </c>
-      <c r="E50" s="78">
+      <c r="E50" s="52">
         <f t="shared" si="2"/>
         <v>-3.6500000000000021</v>
       </c>
-      <c r="F50" s="74">
+      <c r="F50" s="51">
         <f t="shared" si="3"/>
         <v>2.9000000000000137E-2</v>
       </c>
-      <c r="G50" s="63">
+      <c r="G50" s="113">
         <f t="shared" si="4"/>
         <v>-0.10585000000000055</v>
       </c>
-      <c r="H50" s="104"/>
+      <c r="H50" s="114"/>
       <c r="I50" s="27">
         <f t="shared" si="6"/>
         <v>13.322500000000016</v>
@@ -8626,25 +8758,25 @@
       </c>
     </row>
     <row r="51" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="68">
+      <c r="B51" s="45">
         <v>4.8</v>
       </c>
-      <c r="C51" s="69">
+      <c r="C51" s="46">
         <v>0.53</v>
       </c>
-      <c r="E51" s="78">
+      <c r="E51" s="52">
         <f t="shared" si="2"/>
         <v>-3.950000000000002</v>
       </c>
-      <c r="F51" s="74">
+      <c r="F51" s="51">
         <f t="shared" si="3"/>
         <v>-0.20099999999999985</v>
       </c>
-      <c r="G51" s="63">
+      <c r="G51" s="113">
         <f t="shared" si="4"/>
         <v>0.79394999999999982</v>
       </c>
-      <c r="H51" s="104"/>
+      <c r="H51" s="114"/>
       <c r="I51" s="27">
         <f t="shared" si="6"/>
         <v>15.602500000000015</v>
@@ -8655,25 +8787,25 @@
       </c>
     </row>
     <row r="52" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="68">
+      <c r="B52" s="45">
         <v>4</v>
       </c>
-      <c r="C52" s="69">
+      <c r="C52" s="46">
         <v>0.52</v>
       </c>
-      <c r="E52" s="78">
+      <c r="E52" s="52">
         <f t="shared" si="2"/>
         <v>-4.7500000000000018</v>
       </c>
-      <c r="F52" s="74">
+      <c r="F52" s="51">
         <f t="shared" si="3"/>
         <v>-0.21099999999999985</v>
       </c>
-      <c r="G52" s="63">
+      <c r="G52" s="113">
         <f t="shared" si="4"/>
         <v>1.0022499999999996</v>
       </c>
-      <c r="H52" s="104"/>
+      <c r="H52" s="114"/>
       <c r="I52" s="27">
         <f t="shared" si="6"/>
         <v>22.562500000000018</v>
@@ -8684,25 +8816,25 @@
       </c>
     </row>
     <row r="53" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="68">
+      <c r="B53" s="45">
         <v>3.8</v>
       </c>
-      <c r="C53" s="69">
+      <c r="C53" s="46">
         <v>0.43</v>
       </c>
-      <c r="E53" s="78">
+      <c r="E53" s="52">
         <f t="shared" si="2"/>
         <v>-4.950000000000002</v>
       </c>
-      <c r="F53" s="74">
+      <c r="F53" s="51">
         <f t="shared" si="3"/>
         <v>-0.30099999999999988</v>
       </c>
-      <c r="G53" s="63">
+      <c r="G53" s="113">
         <f t="shared" si="4"/>
         <v>1.4899499999999999</v>
       </c>
-      <c r="H53" s="104"/>
+      <c r="H53" s="114"/>
       <c r="I53" s="27">
         <f t="shared" si="6"/>
         <v>24.502500000000019</v>
@@ -8713,25 +8845,25 @@
       </c>
     </row>
     <row r="54" spans="2:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="68">
+      <c r="B54" s="45">
         <v>3.5</v>
       </c>
-      <c r="C54" s="69">
+      <c r="C54" s="46">
         <v>0.5</v>
       </c>
-      <c r="E54" s="78">
+      <c r="E54" s="52">
         <f t="shared" si="2"/>
         <v>-5.2500000000000018</v>
       </c>
-      <c r="F54" s="74">
+      <c r="F54" s="51">
         <f t="shared" si="3"/>
         <v>-0.23099999999999987</v>
       </c>
-      <c r="G54" s="63">
+      <c r="G54" s="113">
         <f t="shared" si="4"/>
         <v>1.2127499999999998</v>
       </c>
-      <c r="H54" s="104"/>
+      <c r="H54" s="114"/>
       <c r="I54" s="27">
         <f t="shared" si="6"/>
         <v>27.562500000000018</v>
@@ -8740,126 +8872,126 @@
         <f t="shared" si="5"/>
         <v>5.3360999999999943E-2</v>
       </c>
-      <c r="L54" s="119" t="s">
+      <c r="L54" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="M54" s="88">
+      <c r="M54" s="57">
         <f>SUM(G43:H72)</f>
         <v>773.87149999999986</v>
       </c>
-      <c r="N54" s="94" t="s">
+      <c r="N54" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="O54" s="95"/>
-      <c r="P54" s="95"/>
-      <c r="Q54" s="95"/>
-      <c r="R54" s="95"/>
-      <c r="S54" s="96"/>
+      <c r="O54" s="133"/>
+      <c r="P54" s="133"/>
+      <c r="Q54" s="133"/>
+      <c r="R54" s="133"/>
+      <c r="S54" s="134"/>
     </row>
     <row r="55" spans="2:19" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B55" s="68">
+      <c r="B55" s="45">
         <v>3.2</v>
       </c>
-      <c r="C55" s="69">
+      <c r="C55" s="46">
         <v>0.45</v>
       </c>
-      <c r="E55" s="115">
+      <c r="E55" s="69">
         <f t="shared" si="2"/>
         <v>-5.5500000000000016</v>
       </c>
-      <c r="F55" s="116">
+      <c r="F55" s="70">
         <f t="shared" si="3"/>
         <v>-0.28099999999999986</v>
       </c>
-      <c r="G55" s="47">
+      <c r="G55" s="96">
         <f t="shared" si="4"/>
         <v>1.5595499999999998</v>
       </c>
-      <c r="H55" s="114"/>
-      <c r="I55" s="117">
+      <c r="H55" s="115"/>
+      <c r="I55" s="71">
         <f t="shared" si="6"/>
         <v>30.802500000000016</v>
       </c>
-      <c r="J55" s="118">
+      <c r="J55" s="72">
         <f t="shared" si="5"/>
         <v>7.896099999999992E-2</v>
       </c>
-      <c r="L55" s="120" t="s">
+      <c r="L55" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="M55" s="121">
+      <c r="M55" s="75">
         <f>SQRT(SUM(I43:I72))</f>
         <v>107.24250556565714</v>
       </c>
-      <c r="N55" s="97"/>
-      <c r="O55" s="98"/>
-      <c r="P55" s="98"/>
-      <c r="Q55" s="98"/>
-      <c r="R55" s="98"/>
-      <c r="S55" s="99"/>
+      <c r="N55" s="135"/>
+      <c r="O55" s="136"/>
+      <c r="P55" s="136"/>
+      <c r="Q55" s="136"/>
+      <c r="R55" s="136"/>
+      <c r="S55" s="137"/>
     </row>
     <row r="56" spans="2:19" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B56" s="68">
+      <c r="B56" s="45">
         <v>3</v>
       </c>
-      <c r="C56" s="69">
+      <c r="C56" s="46">
         <v>0.49</v>
       </c>
-      <c r="E56" s="115">
+      <c r="E56" s="69">
         <f t="shared" si="2"/>
         <v>-5.7500000000000018</v>
       </c>
-      <c r="F56" s="116">
+      <c r="F56" s="70">
         <f t="shared" si="3"/>
         <v>-0.24099999999999988</v>
       </c>
-      <c r="G56" s="47">
+      <c r="G56" s="96">
         <f t="shared" si="4"/>
         <v>1.3857499999999998</v>
       </c>
-      <c r="H56" s="114"/>
-      <c r="I56" s="117">
+      <c r="H56" s="115"/>
+      <c r="I56" s="71">
         <f t="shared" si="6"/>
         <v>33.062500000000021</v>
       </c>
-      <c r="J56" s="118">
+      <c r="J56" s="72">
         <f t="shared" si="5"/>
         <v>5.8080999999999945E-2</v>
       </c>
-      <c r="L56" s="120" t="s">
+      <c r="L56" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="121">
+      <c r="M56" s="75">
         <f>SQRT(SUM(J43:J72))</f>
         <v>7.2852227145091453</v>
       </c>
-      <c r="N56" s="97"/>
-      <c r="O56" s="98"/>
-      <c r="P56" s="98"/>
-      <c r="Q56" s="98"/>
-      <c r="R56" s="98"/>
-      <c r="S56" s="99"/>
+      <c r="N56" s="135"/>
+      <c r="O56" s="136"/>
+      <c r="P56" s="136"/>
+      <c r="Q56" s="136"/>
+      <c r="R56" s="136"/>
+      <c r="S56" s="137"/>
     </row>
     <row r="57" spans="2:19" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B57" s="68">
+      <c r="B57" s="45">
         <v>2.8</v>
       </c>
-      <c r="C57" s="69">
+      <c r="C57" s="46">
         <v>0.47</v>
       </c>
-      <c r="E57" s="78">
+      <c r="E57" s="52">
         <f t="shared" si="2"/>
         <v>-5.950000000000002</v>
       </c>
-      <c r="F57" s="74">
+      <c r="F57" s="51">
         <f t="shared" si="3"/>
         <v>-0.2609999999999999</v>
       </c>
-      <c r="G57" s="63">
+      <c r="G57" s="113">
         <f t="shared" si="4"/>
         <v>1.5529499999999998</v>
       </c>
-      <c r="H57" s="104"/>
+      <c r="H57" s="114"/>
       <c r="I57" s="27">
         <f t="shared" si="6"/>
         <v>35.402500000000025</v>
@@ -8868,40 +9000,40 @@
         <f t="shared" si="5"/>
         <v>6.8120999999999945E-2</v>
       </c>
-      <c r="L57" s="120" t="s">
+      <c r="L57" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="M57" s="121">
+      <c r="M57" s="75">
         <f>M56*M55</f>
         <v>781.28553750779884</v>
       </c>
-      <c r="N57" s="97"/>
-      <c r="O57" s="98"/>
-      <c r="P57" s="98"/>
-      <c r="Q57" s="98"/>
-      <c r="R57" s="98"/>
-      <c r="S57" s="99"/>
+      <c r="N57" s="135"/>
+      <c r="O57" s="136"/>
+      <c r="P57" s="136"/>
+      <c r="Q57" s="136"/>
+      <c r="R57" s="136"/>
+      <c r="S57" s="137"/>
     </row>
     <row r="58" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="70">
+      <c r="B58" s="47">
         <v>2.5</v>
       </c>
-      <c r="C58" s="69">
+      <c r="C58" s="46">
         <v>0.35</v>
       </c>
-      <c r="E58" s="78">
+      <c r="E58" s="52">
         <f t="shared" si="2"/>
         <v>-6.2500000000000018</v>
       </c>
-      <c r="F58" s="74">
+      <c r="F58" s="51">
         <f t="shared" si="3"/>
         <v>-0.38099999999999989</v>
       </c>
-      <c r="G58" s="63">
+      <c r="G58" s="113">
         <f t="shared" si="4"/>
         <v>2.3812500000000001</v>
       </c>
-      <c r="H58" s="104"/>
+      <c r="H58" s="114"/>
       <c r="I58" s="27">
         <f t="shared" si="6"/>
         <v>39.062500000000021</v>
@@ -8910,40 +9042,40 @@
         <f t="shared" si="5"/>
         <v>0.14516099999999993</v>
       </c>
-      <c r="L58" s="122" t="s">
+      <c r="L58" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="M58" s="124">
+      <c r="M58" s="78">
         <f>M54/M57</f>
         <v>0.9905104636501415</v>
       </c>
-      <c r="N58" s="97"/>
-      <c r="O58" s="98"/>
-      <c r="P58" s="98"/>
-      <c r="Q58" s="98"/>
-      <c r="R58" s="98"/>
-      <c r="S58" s="99"/>
+      <c r="N58" s="135"/>
+      <c r="O58" s="136"/>
+      <c r="P58" s="136"/>
+      <c r="Q58" s="136"/>
+      <c r="R58" s="136"/>
+      <c r="S58" s="137"/>
     </row>
     <row r="59" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="68">
+      <c r="B59" s="45">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C59" s="69">
+      <c r="C59" s="46">
         <v>0.33</v>
       </c>
-      <c r="E59" s="78">
+      <c r="E59" s="52">
         <f t="shared" si="2"/>
         <v>-6.450000000000002</v>
       </c>
-      <c r="F59" s="74">
+      <c r="F59" s="51">
         <f t="shared" si="3"/>
         <v>-0.40099999999999986</v>
       </c>
-      <c r="G59" s="63">
+      <c r="G59" s="113">
         <f t="shared" si="4"/>
         <v>2.5864499999999997</v>
       </c>
-      <c r="H59" s="104"/>
+      <c r="H59" s="114"/>
       <c r="I59" s="27">
         <f t="shared" si="6"/>
         <v>41.602500000000028</v>
@@ -8952,40 +9084,40 @@
         <f t="shared" si="5"/>
         <v>0.16080099999999989</v>
       </c>
-      <c r="L59" s="123" t="s">
+      <c r="L59" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="M59" s="125">
+      <c r="M59" s="79">
         <f>CORREL(B43:B72,C43:C72)</f>
         <v>0.9905104636501415</v>
       </c>
-      <c r="N59" s="100"/>
-      <c r="O59" s="101"/>
-      <c r="P59" s="101"/>
-      <c r="Q59" s="101"/>
-      <c r="R59" s="101"/>
-      <c r="S59" s="102"/>
+      <c r="N59" s="138"/>
+      <c r="O59" s="139"/>
+      <c r="P59" s="139"/>
+      <c r="Q59" s="139"/>
+      <c r="R59" s="139"/>
+      <c r="S59" s="140"/>
     </row>
     <row r="60" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="68">
+      <c r="B60" s="45">
         <v>2.1</v>
       </c>
-      <c r="C60" s="69">
+      <c r="C60" s="46">
         <v>0.3</v>
       </c>
-      <c r="E60" s="78">
+      <c r="E60" s="52">
         <f t="shared" si="2"/>
         <v>-6.6500000000000021</v>
       </c>
-      <c r="F60" s="74">
+      <c r="F60" s="51">
         <f t="shared" si="3"/>
         <v>-0.43099999999999988</v>
       </c>
-      <c r="G60" s="63">
+      <c r="G60" s="113">
         <f t="shared" si="4"/>
         <v>2.8661500000000002</v>
       </c>
-      <c r="H60" s="104"/>
+      <c r="H60" s="114"/>
       <c r="I60" s="27">
         <f t="shared" si="6"/>
         <v>44.222500000000025</v>
@@ -8996,25 +9128,25 @@
       </c>
     </row>
     <row r="61" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="71">
+      <c r="B61" s="48">
         <v>2</v>
       </c>
-      <c r="C61" s="69">
+      <c r="C61" s="46">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E61" s="78">
+      <c r="E61" s="52">
         <f t="shared" si="2"/>
         <v>-6.7500000000000018</v>
       </c>
-      <c r="F61" s="74">
+      <c r="F61" s="51">
         <f t="shared" si="3"/>
         <v>-0.45099999999999985</v>
       </c>
-      <c r="G61" s="63">
+      <c r="G61" s="113">
         <f t="shared" si="4"/>
         <v>3.0442499999999999</v>
       </c>
-      <c r="H61" s="104"/>
+      <c r="H61" s="114"/>
       <c r="I61" s="27">
         <f t="shared" si="6"/>
         <v>45.562500000000021</v>
@@ -9023,37 +9155,37 @@
         <f t="shared" si="5"/>
         <v>0.20340099999999986</v>
       </c>
-      <c r="L61" s="129" t="s">
+      <c r="L61" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="M61" s="130"/>
-      <c r="N61" s="130"/>
-      <c r="O61" s="130"/>
-      <c r="P61" s="130"/>
-      <c r="Q61" s="130"/>
-      <c r="R61" s="130"/>
-      <c r="S61" s="131"/>
+      <c r="M61" s="119"/>
+      <c r="N61" s="119"/>
+      <c r="O61" s="119"/>
+      <c r="P61" s="119"/>
+      <c r="Q61" s="119"/>
+      <c r="R61" s="119"/>
+      <c r="S61" s="120"/>
     </row>
     <row r="62" spans="2:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="68">
+      <c r="B62" s="45">
         <v>1.8</v>
       </c>
-      <c r="C62" s="69">
+      <c r="C62" s="46">
         <v>0.25</v>
       </c>
-      <c r="E62" s="78">
+      <c r="E62" s="52">
         <f t="shared" si="2"/>
         <v>-6.950000000000002</v>
       </c>
-      <c r="F62" s="74">
+      <c r="F62" s="51">
         <f t="shared" si="3"/>
         <v>-0.48099999999999987</v>
       </c>
-      <c r="G62" s="63">
+      <c r="G62" s="113">
         <f t="shared" si="4"/>
         <v>3.3429500000000001</v>
       </c>
-      <c r="H62" s="104"/>
+      <c r="H62" s="114"/>
       <c r="I62" s="27">
         <f t="shared" si="6"/>
         <v>48.30250000000003</v>
@@ -9062,37 +9194,37 @@
         <f t="shared" si="5"/>
         <v>0.23136099999999987</v>
       </c>
-      <c r="L62" s="132" t="s">
+      <c r="L62" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="M62" s="133"/>
-      <c r="N62" s="133"/>
-      <c r="O62" s="133"/>
-      <c r="P62" s="133"/>
-      <c r="Q62" s="133"/>
-      <c r="R62" s="133"/>
-      <c r="S62" s="134"/>
+      <c r="M62" s="122"/>
+      <c r="N62" s="122"/>
+      <c r="O62" s="122"/>
+      <c r="P62" s="122"/>
+      <c r="Q62" s="122"/>
+      <c r="R62" s="122"/>
+      <c r="S62" s="123"/>
     </row>
     <row r="63" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="68">
+      <c r="B63" s="45">
         <v>1.7</v>
       </c>
-      <c r="C63" s="69">
+      <c r="C63" s="46">
         <v>0.2</v>
       </c>
-      <c r="E63" s="78">
+      <c r="E63" s="52">
         <f t="shared" si="2"/>
         <v>-7.0500000000000016</v>
       </c>
-      <c r="F63" s="74">
+      <c r="F63" s="51">
         <f t="shared" si="3"/>
         <v>-0.53099999999999992</v>
       </c>
-      <c r="G63" s="63">
+      <c r="G63" s="113">
         <f t="shared" si="4"/>
         <v>3.7435500000000004</v>
       </c>
-      <c r="H63" s="104"/>
+      <c r="H63" s="114"/>
       <c r="I63" s="27">
         <f t="shared" si="6"/>
         <v>49.702500000000022</v>
@@ -9101,35 +9233,35 @@
         <f t="shared" si="5"/>
         <v>0.28196099999999991</v>
       </c>
-      <c r="L63" s="135"/>
-      <c r="M63" s="136"/>
-      <c r="N63" s="136"/>
-      <c r="O63" s="136"/>
-      <c r="P63" s="136"/>
-      <c r="Q63" s="136"/>
-      <c r="R63" s="136"/>
-      <c r="S63" s="137"/>
+      <c r="L63" s="124"/>
+      <c r="M63" s="125"/>
+      <c r="N63" s="125"/>
+      <c r="O63" s="125"/>
+      <c r="P63" s="125"/>
+      <c r="Q63" s="125"/>
+      <c r="R63" s="125"/>
+      <c r="S63" s="126"/>
     </row>
     <row r="64" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B64" s="68">
+      <c r="B64" s="45">
         <v>1.5</v>
       </c>
-      <c r="C64" s="69">
+      <c r="C64" s="46">
         <v>0.22</v>
       </c>
-      <c r="E64" s="78">
+      <c r="E64" s="52">
         <f t="shared" si="2"/>
         <v>-7.2500000000000018</v>
       </c>
-      <c r="F64" s="74">
+      <c r="F64" s="51">
         <f t="shared" si="3"/>
         <v>-0.5109999999999999</v>
       </c>
-      <c r="G64" s="63">
+      <c r="G64" s="113">
         <f t="shared" si="4"/>
         <v>3.7047500000000002</v>
       </c>
-      <c r="H64" s="104"/>
+      <c r="H64" s="114"/>
       <c r="I64" s="27">
         <f t="shared" si="6"/>
         <v>52.562500000000028</v>
@@ -9138,35 +9270,35 @@
         <f t="shared" si="5"/>
         <v>0.26112099999999988</v>
       </c>
-      <c r="L64" s="135"/>
-      <c r="M64" s="136"/>
-      <c r="N64" s="136"/>
-      <c r="O64" s="136"/>
-      <c r="P64" s="136"/>
-      <c r="Q64" s="136"/>
-      <c r="R64" s="136"/>
-      <c r="S64" s="137"/>
-    </row>
-    <row r="65" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B65" s="68">
+      <c r="L64" s="124"/>
+      <c r="M64" s="125"/>
+      <c r="N64" s="125"/>
+      <c r="O64" s="125"/>
+      <c r="P64" s="125"/>
+      <c r="Q64" s="125"/>
+      <c r="R64" s="125"/>
+      <c r="S64" s="126"/>
+    </row>
+    <row r="65" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B65" s="45">
         <v>1.3</v>
       </c>
-      <c r="C65" s="69">
+      <c r="C65" s="46">
         <v>0.13</v>
       </c>
-      <c r="E65" s="78">
+      <c r="E65" s="52">
         <f t="shared" si="2"/>
         <v>-7.450000000000002</v>
       </c>
-      <c r="F65" s="74">
+      <c r="F65" s="51">
         <f t="shared" si="3"/>
         <v>-0.60099999999999987</v>
       </c>
-      <c r="G65" s="63">
+      <c r="G65" s="113">
         <f t="shared" si="4"/>
         <v>4.4774500000000002</v>
       </c>
-      <c r="H65" s="104"/>
+      <c r="H65" s="114"/>
       <c r="I65" s="27">
         <f t="shared" si="6"/>
         <v>55.502500000000026</v>
@@ -9175,35 +9307,35 @@
         <f t="shared" si="5"/>
         <v>0.36120099999999983</v>
       </c>
-      <c r="L65" s="135"/>
-      <c r="M65" s="136"/>
-      <c r="N65" s="136"/>
-      <c r="O65" s="136"/>
-      <c r="P65" s="136"/>
-      <c r="Q65" s="136"/>
-      <c r="R65" s="136"/>
-      <c r="S65" s="137"/>
-    </row>
-    <row r="66" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="68">
+      <c r="L65" s="124"/>
+      <c r="M65" s="125"/>
+      <c r="N65" s="125"/>
+      <c r="O65" s="125"/>
+      <c r="P65" s="125"/>
+      <c r="Q65" s="125"/>
+      <c r="R65" s="125"/>
+      <c r="S65" s="126"/>
+    </row>
+    <row r="66" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="45">
         <v>1.2</v>
       </c>
-      <c r="C66" s="69">
+      <c r="C66" s="46">
         <v>0.08</v>
       </c>
-      <c r="E66" s="78">
+      <c r="E66" s="52">
         <f t="shared" si="2"/>
         <v>-7.5500000000000016</v>
       </c>
-      <c r="F66" s="74">
+      <c r="F66" s="51">
         <f t="shared" si="3"/>
         <v>-0.65099999999999991</v>
       </c>
-      <c r="G66" s="63">
+      <c r="G66" s="113">
         <f t="shared" si="4"/>
         <v>4.9150500000000008</v>
       </c>
-      <c r="H66" s="104"/>
+      <c r="H66" s="114"/>
       <c r="I66" s="27">
         <f t="shared" si="6"/>
         <v>57.002500000000026</v>
@@ -9212,35 +9344,35 @@
         <f t="shared" si="5"/>
         <v>0.42380099999999987</v>
       </c>
-      <c r="L66" s="135"/>
-      <c r="M66" s="136"/>
-      <c r="N66" s="136"/>
-      <c r="O66" s="136"/>
-      <c r="P66" s="136"/>
-      <c r="Q66" s="136"/>
-      <c r="R66" s="136"/>
-      <c r="S66" s="137"/>
-    </row>
-    <row r="67" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B67" s="68">
+      <c r="L66" s="124"/>
+      <c r="M66" s="125"/>
+      <c r="N66" s="125"/>
+      <c r="O66" s="125"/>
+      <c r="P66" s="125"/>
+      <c r="Q66" s="125"/>
+      <c r="R66" s="125"/>
+      <c r="S66" s="126"/>
+    </row>
+    <row r="67" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B67" s="45">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C67" s="69">
+      <c r="C67" s="46">
         <v>0.15</v>
       </c>
-      <c r="E67" s="78">
+      <c r="E67" s="52">
         <f t="shared" si="2"/>
         <v>-7.6500000000000021</v>
       </c>
-      <c r="F67" s="74">
+      <c r="F67" s="51">
         <f t="shared" si="3"/>
         <v>-0.58099999999999985</v>
       </c>
-      <c r="G67" s="63">
+      <c r="G67" s="113">
         <f t="shared" si="4"/>
         <v>4.4446500000000002</v>
       </c>
-      <c r="H67" s="104"/>
+      <c r="H67" s="114"/>
       <c r="I67" s="27">
         <f t="shared" si="6"/>
         <v>58.522500000000029</v>
@@ -9249,35 +9381,35 @@
         <f t="shared" si="5"/>
         <v>0.33756099999999983</v>
       </c>
-      <c r="L67" s="135"/>
-      <c r="M67" s="136"/>
-      <c r="N67" s="136"/>
-      <c r="O67" s="136"/>
-      <c r="P67" s="136"/>
-      <c r="Q67" s="136"/>
-      <c r="R67" s="136"/>
-      <c r="S67" s="137"/>
-    </row>
-    <row r="68" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B68" s="68">
+      <c r="L67" s="124"/>
+      <c r="M67" s="125"/>
+      <c r="N67" s="125"/>
+      <c r="O67" s="125"/>
+      <c r="P67" s="125"/>
+      <c r="Q67" s="125"/>
+      <c r="R67" s="125"/>
+      <c r="S67" s="126"/>
+    </row>
+    <row r="68" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B68" s="45">
         <v>1</v>
       </c>
-      <c r="C68" s="69">
+      <c r="C68" s="46">
         <v>0.05</v>
       </c>
-      <c r="E68" s="78">
+      <c r="E68" s="52">
         <f t="shared" si="2"/>
         <v>-7.7500000000000018</v>
       </c>
-      <c r="F68" s="74">
+      <c r="F68" s="51">
         <f t="shared" si="3"/>
         <v>-0.68099999999999983</v>
       </c>
-      <c r="G68" s="63">
+      <c r="G68" s="113">
         <f t="shared" si="4"/>
         <v>5.2777500000000002</v>
       </c>
-      <c r="H68" s="104"/>
+      <c r="H68" s="114"/>
       <c r="I68" s="27">
         <f t="shared" si="6"/>
         <v>60.062500000000028</v>
@@ -9286,35 +9418,35 @@
         <f t="shared" si="5"/>
         <v>0.46376099999999976</v>
       </c>
-      <c r="L68" s="135"/>
-      <c r="M68" s="136"/>
-      <c r="N68" s="136"/>
-      <c r="O68" s="136"/>
-      <c r="P68" s="136"/>
-      <c r="Q68" s="136"/>
-      <c r="R68" s="136"/>
-      <c r="S68" s="137"/>
-    </row>
-    <row r="69" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B69" s="68">
+      <c r="L68" s="124"/>
+      <c r="M68" s="125"/>
+      <c r="N68" s="125"/>
+      <c r="O68" s="125"/>
+      <c r="P68" s="125"/>
+      <c r="Q68" s="125"/>
+      <c r="R68" s="125"/>
+      <c r="S68" s="126"/>
+    </row>
+    <row r="69" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="45">
         <v>0.9</v>
       </c>
-      <c r="C69" s="69">
+      <c r="C69" s="46">
         <v>0.08</v>
       </c>
-      <c r="E69" s="78">
+      <c r="E69" s="52">
         <f t="shared" si="2"/>
         <v>-7.8500000000000014</v>
       </c>
-      <c r="F69" s="74">
+      <c r="F69" s="51">
         <f t="shared" si="3"/>
         <v>-0.65099999999999991</v>
       </c>
-      <c r="G69" s="63">
+      <c r="G69" s="113">
         <f t="shared" si="4"/>
         <v>5.1103500000000004</v>
       </c>
-      <c r="H69" s="104"/>
+      <c r="H69" s="114"/>
       <c r="I69" s="27">
         <f t="shared" si="6"/>
         <v>61.622500000000024</v>
@@ -9323,35 +9455,35 @@
         <f t="shared" si="5"/>
         <v>0.42380099999999987</v>
       </c>
-      <c r="L69" s="135"/>
-      <c r="M69" s="136"/>
-      <c r="N69" s="136"/>
-      <c r="O69" s="136"/>
-      <c r="P69" s="136"/>
-      <c r="Q69" s="136"/>
-      <c r="R69" s="136"/>
-      <c r="S69" s="137"/>
-    </row>
-    <row r="70" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B70" s="68">
+      <c r="L69" s="124"/>
+      <c r="M69" s="125"/>
+      <c r="N69" s="125"/>
+      <c r="O69" s="125"/>
+      <c r="P69" s="125"/>
+      <c r="Q69" s="125"/>
+      <c r="R69" s="125"/>
+      <c r="S69" s="126"/>
+    </row>
+    <row r="70" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="45">
         <v>0.8</v>
       </c>
-      <c r="C70" s="69">
+      <c r="C70" s="46">
         <v>0.04</v>
       </c>
-      <c r="E70" s="78">
+      <c r="E70" s="52">
         <f t="shared" si="2"/>
         <v>-7.950000000000002</v>
       </c>
-      <c r="F70" s="74">
+      <c r="F70" s="51">
         <f t="shared" si="3"/>
         <v>-0.69099999999999984</v>
       </c>
-      <c r="G70" s="63">
+      <c r="G70" s="113">
         <f t="shared" si="4"/>
         <v>5.4934500000000002</v>
       </c>
-      <c r="H70" s="104"/>
+      <c r="H70" s="114"/>
       <c r="I70" s="27">
         <f t="shared" si="6"/>
         <v>63.202500000000029</v>
@@ -9360,35 +9492,35 @@
         <f t="shared" si="5"/>
         <v>0.47748099999999977</v>
       </c>
-      <c r="L70" s="135"/>
-      <c r="M70" s="136"/>
-      <c r="N70" s="136"/>
-      <c r="O70" s="136"/>
-      <c r="P70" s="136"/>
-      <c r="Q70" s="136"/>
-      <c r="R70" s="136"/>
-      <c r="S70" s="137"/>
-    </row>
-    <row r="71" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B71" s="68">
+      <c r="L70" s="124"/>
+      <c r="M70" s="125"/>
+      <c r="N70" s="125"/>
+      <c r="O70" s="125"/>
+      <c r="P70" s="125"/>
+      <c r="Q70" s="125"/>
+      <c r="R70" s="125"/>
+      <c r="S70" s="126"/>
+    </row>
+    <row r="71" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B71" s="45">
         <v>0.7</v>
       </c>
-      <c r="C71" s="69">
+      <c r="C71" s="46">
         <v>0.01</v>
       </c>
-      <c r="E71" s="78">
+      <c r="E71" s="52">
         <f t="shared" si="2"/>
         <v>-8.0500000000000025</v>
       </c>
-      <c r="F71" s="74">
+      <c r="F71" s="51">
         <f t="shared" si="3"/>
         <v>-0.72099999999999986</v>
       </c>
-      <c r="G71" s="63">
+      <c r="G71" s="113">
         <f t="shared" si="4"/>
         <v>5.804050000000001</v>
       </c>
-      <c r="H71" s="104"/>
+      <c r="H71" s="114"/>
       <c r="I71" s="27">
         <f t="shared" si="6"/>
         <v>64.802500000000038</v>
@@ -9397,54 +9529,1597 @@
         <f t="shared" si="5"/>
         <v>0.51984099999999978</v>
       </c>
-      <c r="L71" s="135"/>
-      <c r="M71" s="136"/>
-      <c r="N71" s="136"/>
-      <c r="O71" s="136"/>
-      <c r="P71" s="136"/>
-      <c r="Q71" s="136"/>
-      <c r="R71" s="136"/>
-      <c r="S71" s="137"/>
-    </row>
-    <row r="72" spans="2:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="72">
+      <c r="L71" s="124"/>
+      <c r="M71" s="125"/>
+      <c r="N71" s="125"/>
+      <c r="O71" s="125"/>
+      <c r="P71" s="125"/>
+      <c r="Q71" s="125"/>
+      <c r="R71" s="125"/>
+      <c r="S71" s="126"/>
+    </row>
+    <row r="72" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="49">
         <v>0.6</v>
       </c>
-      <c r="C72" s="73">
+      <c r="C72" s="50">
         <v>0.01</v>
       </c>
-      <c r="E72" s="79">
+      <c r="E72" s="53">
         <f t="shared" si="2"/>
         <v>-8.1500000000000021</v>
       </c>
-      <c r="F72" s="80">
+      <c r="F72" s="54">
         <f t="shared" si="3"/>
         <v>-0.72099999999999986</v>
       </c>
-      <c r="G72" s="81">
+      <c r="G72" s="116">
         <f t="shared" si="4"/>
         <v>5.87615</v>
       </c>
-      <c r="H72" s="105"/>
-      <c r="I72" s="112">
+      <c r="H72" s="117"/>
+      <c r="I72" s="67">
         <f t="shared" si="6"/>
         <v>66.422500000000028</v>
       </c>
-      <c r="J72" s="113">
+      <c r="J72" s="68">
         <f t="shared" si="5"/>
         <v>0.51984099999999978</v>
       </c>
-      <c r="L72" s="138"/>
-      <c r="M72" s="139"/>
-      <c r="N72" s="139"/>
-      <c r="O72" s="139"/>
-      <c r="P72" s="139"/>
-      <c r="Q72" s="139"/>
-      <c r="R72" s="139"/>
-      <c r="S72" s="140"/>
+      <c r="L72" s="127"/>
+      <c r="M72" s="128"/>
+      <c r="N72" s="128"/>
+      <c r="O72" s="128"/>
+      <c r="P72" s="128"/>
+      <c r="Q72" s="128"/>
+      <c r="R72" s="128"/>
+      <c r="S72" s="129"/>
+    </row>
+    <row r="75" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="92"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="92"/>
+      <c r="H76" s="93"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="157" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="158"/>
+      <c r="C77" s="158"/>
+      <c r="D77" s="158"/>
+      <c r="E77" s="158"/>
+      <c r="F77" s="158"/>
+      <c r="G77" s="158"/>
+      <c r="H77" s="159"/>
+    </row>
+    <row r="78" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="156"/>
+      <c r="B78" s="164"/>
+      <c r="C78" s="164"/>
+      <c r="D78" s="164"/>
+      <c r="E78" s="164"/>
+      <c r="F78" s="164"/>
+      <c r="G78" s="164"/>
+      <c r="H78" s="165"/>
+    </row>
+    <row r="79" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="160" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="161" t="s">
+        <v>98</v>
+      </c>
+      <c r="C79" s="161" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="161" t="s">
+        <v>43</v>
+      </c>
+      <c r="E79" s="161" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" s="161" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="H79" s="161" t="s">
+        <v>45</v>
+      </c>
+      <c r="I79" s="161" t="s">
+        <v>96</v>
+      </c>
+      <c r="J79" s="161" t="s">
+        <v>91</v>
+      </c>
+      <c r="K79" s="161" t="s">
+        <v>92</v>
+      </c>
+      <c r="L79" s="161" t="s">
+        <v>93</v>
+      </c>
+      <c r="M79" s="161" t="s">
+        <v>94</v>
+      </c>
+      <c r="N79" s="161" t="s">
+        <v>95</v>
+      </c>
+      <c r="O79" s="162" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="151" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="150">
+        <v>3.2</v>
+      </c>
+      <c r="C80" s="150">
+        <v>0.45</v>
+      </c>
+      <c r="D80" s="150">
+        <v>12.9</v>
+      </c>
+      <c r="E80" s="150">
+        <v>31</v>
+      </c>
+      <c r="F80" s="150">
+        <v>52</v>
+      </c>
+      <c r="G80" s="150">
+        <v>48</v>
+      </c>
+      <c r="H80" s="150">
+        <v>0.7</v>
+      </c>
+      <c r="I80" s="150">
+        <v>3.8445285796830801</v>
+      </c>
+      <c r="J80" s="150">
+        <v>5.3798605929893757</v>
+      </c>
+      <c r="K80" s="150">
+        <v>14.05625839261644</v>
+      </c>
+      <c r="L80" s="150">
+        <v>5.4403033003684644</v>
+      </c>
+      <c r="M80" s="150">
+        <v>19.643533287064219</v>
+      </c>
+      <c r="N80" s="150">
+        <v>1.764227876437735</v>
+      </c>
+      <c r="O80" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81" s="151" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="150">
+        <v>1.5</v>
+      </c>
+      <c r="C81" s="150">
+        <v>0.22</v>
+      </c>
+      <c r="D81" s="150">
+        <v>15.7</v>
+      </c>
+      <c r="E81" s="150">
+        <v>27</v>
+      </c>
+      <c r="F81" s="150">
+        <v>51</v>
+      </c>
+      <c r="G81" s="150">
+        <v>49</v>
+      </c>
+      <c r="H81" s="150">
+        <v>0.3</v>
+      </c>
+      <c r="I81" s="150">
+        <v>1.911151485361638</v>
+      </c>
+      <c r="J81" s="150">
+        <v>0</v>
+      </c>
+      <c r="K81" s="150">
+        <v>16.057400163164651</v>
+      </c>
+      <c r="L81" s="150">
+        <v>2.238213573366044</v>
+      </c>
+      <c r="M81" s="150">
+        <v>21.69493258804922</v>
+      </c>
+      <c r="N81" s="150">
+        <v>4.5407488369210647</v>
+      </c>
+      <c r="O81" s="152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82" s="151" t="s">
+        <v>30</v>
+      </c>
+      <c r="B82" s="150">
+        <v>3.5</v>
+      </c>
+      <c r="C82" s="150">
+        <v>0.5</v>
+      </c>
+      <c r="D82" s="150">
+        <v>13</v>
+      </c>
+      <c r="E82" s="150">
+        <v>30</v>
+      </c>
+      <c r="F82" s="150">
+        <v>51</v>
+      </c>
+      <c r="G82" s="150">
+        <v>49</v>
+      </c>
+      <c r="H82" s="150">
+        <v>0.8</v>
+      </c>
+      <c r="I82" s="150">
+        <v>2.7876334048794869</v>
+      </c>
+      <c r="J82" s="150">
+        <v>4.5407488369210647</v>
+      </c>
+      <c r="K82" s="150">
+        <v>13.5673468297969</v>
+      </c>
+      <c r="L82" s="150">
+        <v>4.2221321627822119</v>
+      </c>
+      <c r="M82" s="150">
+        <v>19.349493533423551</v>
+      </c>
+      <c r="N82" s="150">
+        <v>0</v>
+      </c>
+      <c r="O82" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A83" s="151" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83" s="150">
+        <v>1.2</v>
+      </c>
+      <c r="C83" s="150">
+        <v>0.08</v>
+      </c>
+      <c r="D83" s="150">
+        <v>14</v>
+      </c>
+      <c r="E83" s="150">
+        <v>27</v>
+      </c>
+      <c r="F83" s="150">
+        <v>50</v>
+      </c>
+      <c r="G83" s="150">
+        <v>50</v>
+      </c>
+      <c r="H83" s="150">
+        <v>0.2</v>
+      </c>
+      <c r="I83" s="150">
+        <v>2.5518816586981461</v>
+      </c>
+      <c r="J83" s="150">
+        <v>2.238213573366044</v>
+      </c>
+      <c r="K83" s="150">
+        <v>16.175676183702489</v>
+      </c>
+      <c r="L83" s="150">
+        <v>0</v>
+      </c>
+      <c r="M83" s="150">
+        <v>22.070398727707659</v>
+      </c>
+      <c r="N83" s="150">
+        <v>4.2221321627822119</v>
+      </c>
+      <c r="O83" s="152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A84" s="151" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" s="150">
+        <v>2</v>
+      </c>
+      <c r="C84" s="150">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D84" s="150">
+        <v>16.5</v>
+      </c>
+      <c r="E84" s="150">
+        <v>29</v>
+      </c>
+      <c r="F84" s="150">
+        <v>51</v>
+      </c>
+      <c r="G84" s="150">
+        <v>49</v>
+      </c>
+      <c r="H84" s="150">
+        <v>0.5</v>
+      </c>
+      <c r="I84" s="150">
+        <v>2.1391820866864042</v>
+      </c>
+      <c r="J84" s="150">
+        <v>2.2211708624056818</v>
+      </c>
+      <c r="K84" s="150">
+        <v>15.604887055022219</v>
+      </c>
+      <c r="L84" s="150">
+        <v>3.6083237105337429</v>
+      </c>
+      <c r="M84" s="150">
+        <v>21.069943046909259</v>
+      </c>
+      <c r="N84" s="150">
+        <v>3.95454169278818</v>
+      </c>
+      <c r="O84" s="152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85" s="151" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" s="150">
+        <v>10.5</v>
+      </c>
+      <c r="C85" s="150">
+        <v>1.03</v>
+      </c>
+      <c r="D85" s="150">
+        <v>10.9</v>
+      </c>
+      <c r="E85" s="150">
+        <v>30</v>
+      </c>
+      <c r="F85" s="150">
+        <v>51</v>
+      </c>
+      <c r="G85" s="150">
+        <v>49</v>
+      </c>
+      <c r="H85" s="150">
+        <v>2.8</v>
+      </c>
+      <c r="I85" s="150">
+        <v>9.1462341977449935</v>
+      </c>
+      <c r="J85" s="150">
+        <v>10.951990686628619</v>
+      </c>
+      <c r="K85" s="150">
+        <v>6.5627738038119228</v>
+      </c>
+      <c r="L85" s="150">
+        <v>10.71272607696099</v>
+      </c>
+      <c r="M85" s="150">
+        <v>12.46675579290779</v>
+      </c>
+      <c r="N85" s="150">
+        <v>7.5954525869101444</v>
+      </c>
+      <c r="O85" s="152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86" s="151" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" s="150">
+        <v>16.8</v>
+      </c>
+      <c r="C86" s="150">
+        <v>1.23</v>
+      </c>
+      <c r="D86" s="150">
+        <v>12.4</v>
+      </c>
+      <c r="E86" s="150">
+        <v>29</v>
+      </c>
+      <c r="F86" s="150">
+        <v>51</v>
+      </c>
+      <c r="G86" s="150">
+        <v>49</v>
+      </c>
+      <c r="H86" s="150">
+        <v>3.1</v>
+      </c>
+      <c r="I86" s="150">
+        <v>14.477140601651969</v>
+      </c>
+      <c r="J86" s="150">
+        <v>16.057400163164651</v>
+      </c>
+      <c r="K86" s="150">
+        <v>0</v>
+      </c>
+      <c r="L86" s="150">
+        <v>16.175676183702489</v>
+      </c>
+      <c r="M86" s="150">
+        <v>6.2072538211353958</v>
+      </c>
+      <c r="N86" s="150">
+        <v>13.5673468297969</v>
+      </c>
+      <c r="O86" s="152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="151" t="s">
+        <v>26</v>
+      </c>
+      <c r="B87" s="150">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C87" s="150">
+        <v>0.15</v>
+      </c>
+      <c r="D87" s="150">
+        <v>11.5</v>
+      </c>
+      <c r="E87" s="150">
+        <v>29</v>
+      </c>
+      <c r="F87" s="150">
+        <v>51</v>
+      </c>
+      <c r="G87" s="150">
+        <v>49</v>
+      </c>
+      <c r="H87" s="150">
+        <v>0.2</v>
+      </c>
+      <c r="I87" s="150">
+        <v>3.8784532999637888</v>
+      </c>
+      <c r="J87" s="150">
+        <v>4.6706423541093356</v>
+      </c>
+      <c r="K87" s="150">
+        <v>16.027364100188159</v>
+      </c>
+      <c r="L87" s="150">
+        <v>3.502127924562437</v>
+      </c>
+      <c r="M87" s="150">
+        <v>21.96147536027577</v>
+      </c>
+      <c r="N87" s="150">
+        <v>3.0809901006007792</v>
+      </c>
+      <c r="O87" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88" s="151" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="150">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C88" s="150">
+        <v>0.33</v>
+      </c>
+      <c r="D88" s="150">
+        <v>15.2</v>
+      </c>
+      <c r="E88" s="150">
+        <v>31</v>
+      </c>
+      <c r="F88" s="150">
+        <v>52</v>
+      </c>
+      <c r="G88" s="150">
+        <v>48</v>
+      </c>
+      <c r="H88" s="150">
+        <v>0.5</v>
+      </c>
+      <c r="I88" s="150">
+        <v>3.3822477733010632</v>
+      </c>
+      <c r="J88" s="150">
+        <v>4.3522522904813323</v>
+      </c>
+      <c r="K88" s="150">
+        <v>15.22038107275899</v>
+      </c>
+      <c r="L88" s="150">
+        <v>5.1771130951525484</v>
+      </c>
+      <c r="M88" s="150">
+        <v>20.597815418145679</v>
+      </c>
+      <c r="N88" s="150">
+        <v>3.0657625478826631</v>
+      </c>
+      <c r="O88" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89" s="151" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" s="150">
+        <v>2.8</v>
+      </c>
+      <c r="C89" s="150">
+        <v>0.47</v>
+      </c>
+      <c r="D89" s="150">
+        <v>14.8</v>
+      </c>
+      <c r="E89" s="150">
+        <v>28</v>
+      </c>
+      <c r="F89" s="150">
+        <v>51</v>
+      </c>
+      <c r="G89" s="150">
+        <v>49</v>
+      </c>
+      <c r="H89" s="150">
+        <v>0.6</v>
+      </c>
+      <c r="I89" s="150">
+        <v>0</v>
+      </c>
+      <c r="J89" s="150">
+        <v>1.911151485361638</v>
+      </c>
+      <c r="K89" s="150">
+        <v>14.477140601651969</v>
+      </c>
+      <c r="L89" s="150">
+        <v>2.5518816586981461</v>
+      </c>
+      <c r="M89" s="150">
+        <v>20.17963329696553</v>
+      </c>
+      <c r="N89" s="150">
+        <v>2.7876334048794869</v>
+      </c>
+      <c r="O89" s="152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90" s="151" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="150">
+        <v>1.7</v>
+      </c>
+      <c r="C90" s="150">
+        <v>0.2</v>
+      </c>
+      <c r="D90" s="150">
+        <v>17.5</v>
+      </c>
+      <c r="E90" s="150">
+        <v>28</v>
+      </c>
+      <c r="F90" s="150">
+        <v>51</v>
+      </c>
+      <c r="G90" s="150">
+        <v>49</v>
+      </c>
+      <c r="H90" s="150">
+        <v>0.4</v>
+      </c>
+      <c r="I90" s="150">
+        <v>2.9347742672989341</v>
+      </c>
+      <c r="J90" s="150">
+        <v>2.0713280763799831</v>
+      </c>
+      <c r="K90" s="150">
+        <v>16.228706048234411</v>
+      </c>
+      <c r="L90" s="150">
+        <v>3.9439066926082309</v>
+      </c>
+      <c r="M90" s="150">
+        <v>21.604187094172271</v>
+      </c>
+      <c r="N90" s="150">
+        <v>5.2668776329054774</v>
+      </c>
+      <c r="O90" s="152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91" s="151" t="s">
+        <v>101</v>
+      </c>
+      <c r="B91" s="150">
+        <v>4</v>
+      </c>
+      <c r="C91" s="150">
+        <v>0.52</v>
+      </c>
+      <c r="D91" s="150">
+        <v>11.6</v>
+      </c>
+      <c r="E91" s="150">
+        <v>29</v>
+      </c>
+      <c r="F91" s="150">
+        <v>51</v>
+      </c>
+      <c r="G91" s="150">
+        <v>49</v>
+      </c>
+      <c r="H91" s="150">
+        <v>0.9</v>
+      </c>
+      <c r="I91" s="150">
+        <v>3.5738634557016882</v>
+      </c>
+      <c r="J91" s="150">
+        <v>5.2449976167773418</v>
+      </c>
+      <c r="K91" s="150">
+        <v>13.031657607534051</v>
+      </c>
+      <c r="L91" s="150">
+        <v>4.5037317859748267</v>
+      </c>
+      <c r="M91" s="150">
+        <v>18.979307152791431</v>
+      </c>
+      <c r="N91" s="150">
+        <v>1.794547296674011</v>
+      </c>
+      <c r="O91" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92" s="151" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="150">
+        <v>2.5</v>
+      </c>
+      <c r="C92" s="150">
+        <v>0.35</v>
+      </c>
+      <c r="D92" s="150">
+        <v>14.1</v>
+      </c>
+      <c r="E92" s="150">
+        <v>30</v>
+      </c>
+      <c r="F92" s="150">
+        <v>52</v>
+      </c>
+      <c r="G92" s="150">
+        <v>48</v>
+      </c>
+      <c r="H92" s="150">
+        <v>0.6</v>
+      </c>
+      <c r="I92" s="150">
+        <v>2.567956385922471</v>
+      </c>
+      <c r="J92" s="150">
+        <v>3.8297388944939841</v>
+      </c>
+      <c r="K92" s="150">
+        <v>14.74463970397378</v>
+      </c>
+      <c r="L92" s="150">
+        <v>4.3511952380926324</v>
+      </c>
+      <c r="M92" s="150">
+        <v>20.312419845995699</v>
+      </c>
+      <c r="N92" s="150">
+        <v>2.0670026608594392</v>
+      </c>
+      <c r="O92" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93" s="151" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="150">
+        <v>1</v>
+      </c>
+      <c r="C93" s="150">
+        <v>0.05</v>
+      </c>
+      <c r="D93" s="150">
+        <v>13.6</v>
+      </c>
+      <c r="E93" s="150">
+        <v>26</v>
+      </c>
+      <c r="F93" s="150">
+        <v>51</v>
+      </c>
+      <c r="G93" s="150">
+        <v>49</v>
+      </c>
+      <c r="H93" s="150">
+        <v>0.1</v>
+      </c>
+      <c r="I93" s="150">
+        <v>3.017681229023371</v>
+      </c>
+      <c r="J93" s="150">
+        <v>2.3935120638927221</v>
+      </c>
+      <c r="K93" s="150">
+        <v>16.446045117291881</v>
+      </c>
+      <c r="L93" s="150">
+        <v>1.7918984346217841</v>
+      </c>
+      <c r="M93" s="150">
+        <v>22.306106787155841</v>
+      </c>
+      <c r="N93" s="150">
+        <v>4.8272663071349191</v>
+      </c>
+      <c r="O93" s="152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="150">
+        <v>103.5</v>
+      </c>
+      <c r="C94" s="150">
+        <v>7.18</v>
+      </c>
+      <c r="D94" s="150">
+        <v>10.5</v>
+      </c>
+      <c r="E94" s="150">
+        <v>32</v>
+      </c>
+      <c r="F94" s="150">
+        <v>52</v>
+      </c>
+      <c r="G94" s="150">
+        <v>48</v>
+      </c>
+      <c r="H94" s="150">
+        <v>18</v>
+      </c>
+      <c r="I94" s="150">
+        <v>102.59027293072189</v>
+      </c>
+      <c r="J94" s="150">
+        <v>104.0181311118403</v>
+      </c>
+      <c r="K94" s="150">
+        <v>88.254815732627307</v>
+      </c>
+      <c r="L94" s="150">
+        <v>104.29664424131779</v>
+      </c>
+      <c r="M94" s="150">
+        <v>82.504802890498439</v>
+      </c>
+      <c r="N94" s="150">
+        <v>101.74827959233509</v>
+      </c>
+      <c r="O94" s="152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95" s="151" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" s="150">
+        <v>44.1</v>
+      </c>
+      <c r="C95" s="150">
+        <v>2.57</v>
+      </c>
+      <c r="D95" s="150">
+        <v>11.2</v>
+      </c>
+      <c r="E95" s="150">
+        <v>31</v>
+      </c>
+      <c r="F95" s="150">
+        <v>53</v>
+      </c>
+      <c r="G95" s="150">
+        <v>47</v>
+      </c>
+      <c r="H95" s="150">
+        <v>7.5</v>
+      </c>
+      <c r="I95" s="150">
+        <v>42.280846727566853</v>
+      </c>
+      <c r="J95" s="150">
+        <v>43.776392039545698</v>
+      </c>
+      <c r="K95" s="150">
+        <v>27.92643192389605</v>
+      </c>
+      <c r="L95" s="150">
+        <v>44.065180131255559</v>
+      </c>
+      <c r="M95" s="150">
+        <v>22.173308278197911</v>
+      </c>
+      <c r="N95" s="150">
+        <v>41.349424421628903</v>
+      </c>
+      <c r="O95" s="152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A96" s="151" t="s">
+        <v>25</v>
+      </c>
+      <c r="B96" s="150">
+        <v>1.3</v>
+      </c>
+      <c r="C96" s="150">
+        <v>0.13</v>
+      </c>
+      <c r="D96" s="150">
+        <v>18.2</v>
+      </c>
+      <c r="E96" s="150">
+        <v>26</v>
+      </c>
+      <c r="F96" s="150">
+        <v>52</v>
+      </c>
+      <c r="G96" s="150">
+        <v>48</v>
+      </c>
+      <c r="H96" s="150">
+        <v>0.3</v>
+      </c>
+      <c r="I96" s="150">
+        <v>4.473879748048665</v>
+      </c>
+      <c r="J96" s="150">
+        <v>3.0492786032109298</v>
+      </c>
+      <c r="K96" s="150">
+        <v>17.144678474675459</v>
+      </c>
+      <c r="L96" s="150">
+        <v>5.1635743434175509</v>
+      </c>
+      <c r="M96" s="150">
+        <v>22.364927900621542</v>
+      </c>
+      <c r="N96" s="150">
+        <v>7.0899153732608111</v>
+      </c>
+      <c r="O96" s="152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A97" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97" s="150">
+        <v>3.8</v>
+      </c>
+      <c r="C97" s="150">
+        <v>0.43</v>
+      </c>
+      <c r="D97" s="150">
+        <v>10.7</v>
+      </c>
+      <c r="E97" s="150">
+        <v>32</v>
+      </c>
+      <c r="F97" s="150">
+        <v>53</v>
+      </c>
+      <c r="G97" s="150">
+        <v>47</v>
+      </c>
+      <c r="H97" s="150">
+        <v>0.8</v>
+      </c>
+      <c r="I97" s="150">
+        <v>6.4692812583779364</v>
+      </c>
+      <c r="J97" s="150">
+        <v>7.9739638825367152</v>
+      </c>
+      <c r="K97" s="150">
+        <v>13.95779352190023</v>
+      </c>
+      <c r="L97" s="150">
+        <v>7.8187275179532891</v>
+      </c>
+      <c r="M97" s="150">
+        <v>19.400257730246778</v>
+      </c>
+      <c r="N97" s="150">
+        <v>4.169520356108122</v>
+      </c>
+      <c r="O97" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A98" s="151" t="s">
+        <v>22</v>
+      </c>
+      <c r="B98" s="150">
+        <v>1.8</v>
+      </c>
+      <c r="C98" s="150">
+        <v>0.25</v>
+      </c>
+      <c r="D98" s="150">
+        <v>10</v>
+      </c>
+      <c r="E98" s="150">
+        <v>31</v>
+      </c>
+      <c r="F98" s="150">
+        <v>52</v>
+      </c>
+      <c r="G98" s="150">
+        <v>48</v>
+      </c>
+      <c r="H98" s="150">
+        <v>0.4</v>
+      </c>
+      <c r="I98" s="150">
+        <v>5.9269216293114599</v>
+      </c>
+      <c r="J98" s="150">
+        <v>7.1127280279791378</v>
+      </c>
+      <c r="K98" s="150">
+        <v>15.652808054786849</v>
+      </c>
+      <c r="L98" s="150">
+        <v>6.3583724332568003</v>
+      </c>
+      <c r="M98" s="150">
+        <v>21.40468173087374</v>
+      </c>
+      <c r="N98" s="150">
+        <v>3.8874799034850329</v>
+      </c>
+      <c r="O98" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A99" s="151" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" s="150">
+        <v>2.1</v>
+      </c>
+      <c r="C99" s="150">
+        <v>0.3</v>
+      </c>
+      <c r="D99" s="150">
+        <v>13.3</v>
+      </c>
+      <c r="E99" s="150">
+        <v>32</v>
+      </c>
+      <c r="F99" s="150">
+        <v>53</v>
+      </c>
+      <c r="G99" s="150">
+        <v>47</v>
+      </c>
+      <c r="H99" s="150">
+        <v>0.5</v>
+      </c>
+      <c r="I99" s="150">
+        <v>5.1748333306494034</v>
+      </c>
+      <c r="J99" s="150">
+        <v>6.2583064801909458</v>
+      </c>
+      <c r="K99" s="150">
+        <v>15.541071391638351</v>
+      </c>
+      <c r="L99" s="150">
+        <v>6.6662133179189524</v>
+      </c>
+      <c r="M99" s="150">
+        <v>20.874743112191819</v>
+      </c>
+      <c r="N99" s="150">
+        <v>3.765634076752546</v>
+      </c>
+      <c r="O99" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A100" s="151" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="150">
+        <v>6.2</v>
+      </c>
+      <c r="C100" s="150">
+        <v>0.48</v>
+      </c>
+      <c r="D100" s="150">
+        <v>12</v>
+      </c>
+      <c r="E100" s="150">
+        <v>32</v>
+      </c>
+      <c r="F100" s="150">
+        <v>52</v>
+      </c>
+      <c r="G100" s="150">
+        <v>48</v>
+      </c>
+      <c r="H100" s="150">
+        <v>1.3</v>
+      </c>
+      <c r="I100" s="150">
+        <v>6.1554934814359124</v>
+      </c>
+      <c r="J100" s="150">
+        <v>7.9904693228871109</v>
+      </c>
+      <c r="K100" s="150">
+        <v>11.283727221091439</v>
+      </c>
+      <c r="L100" s="150">
+        <v>7.9605276207045472</v>
+      </c>
+      <c r="M100" s="150">
+        <v>16.767602690903669</v>
+      </c>
+      <c r="N100" s="150">
+        <v>3.8131876429045559</v>
+      </c>
+      <c r="O100" s="152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A101" s="151" t="s">
+        <v>29</v>
+      </c>
+      <c r="B101" s="150">
+        <v>0.7</v>
+      </c>
+      <c r="C101" s="150">
+        <v>0.01</v>
+      </c>
+      <c r="D101" s="150">
+        <v>20</v>
+      </c>
+      <c r="E101" s="150">
+        <v>25</v>
+      </c>
+      <c r="F101" s="150">
+        <v>51</v>
+      </c>
+      <c r="G101" s="150">
+        <v>49</v>
+      </c>
+      <c r="H101" s="150">
+        <v>0.05</v>
+      </c>
+      <c r="I101" s="150">
+        <v>6.4003203044847679</v>
+      </c>
+      <c r="J101" s="150">
+        <v>4.8204356649580964</v>
+      </c>
+      <c r="K101" s="150">
+        <v>18.540790166549002</v>
+      </c>
+      <c r="L101" s="150">
+        <v>6.5021073506979246</v>
+      </c>
+      <c r="M101" s="150">
+        <v>23.632200490009389</v>
+      </c>
+      <c r="N101" s="150">
+        <v>9.0907975447702061</v>
+      </c>
+      <c r="O101" s="152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A102" s="151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="150">
+        <v>22.4</v>
+      </c>
+      <c r="C102" s="150">
+        <v>2.23</v>
+      </c>
+      <c r="D102" s="150">
+        <v>13.8</v>
+      </c>
+      <c r="E102" s="150">
+        <v>30</v>
+      </c>
+      <c r="F102" s="150">
+        <v>52</v>
+      </c>
+      <c r="G102" s="150">
+        <v>48</v>
+      </c>
+      <c r="H102" s="150">
+        <v>4.2</v>
+      </c>
+      <c r="I102" s="150">
+        <v>20.17963329696553</v>
+      </c>
+      <c r="J102" s="150">
+        <v>21.69493258804922</v>
+      </c>
+      <c r="K102" s="150">
+        <v>6.2072538211353958</v>
+      </c>
+      <c r="L102" s="150">
+        <v>22.070398727707659</v>
+      </c>
+      <c r="M102" s="150">
+        <v>0</v>
+      </c>
+      <c r="N102" s="150">
+        <v>19.349493533423551</v>
+      </c>
+      <c r="O102" s="152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="153" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="154">
+        <v>3</v>
+      </c>
+      <c r="C103" s="154">
+        <v>0.49</v>
+      </c>
+      <c r="D103" s="154">
+        <v>13.5</v>
+      </c>
+      <c r="E103" s="154">
+        <v>29</v>
+      </c>
+      <c r="F103" s="154">
+        <v>51</v>
+      </c>
+      <c r="G103" s="154">
+        <v>49</v>
+      </c>
+      <c r="H103" s="154">
+        <v>0.7</v>
+      </c>
+      <c r="I103" s="154">
+        <v>1.655415355734023</v>
+      </c>
+      <c r="J103" s="154">
+        <v>3.3649517084201959</v>
+      </c>
+      <c r="K103" s="154">
+        <v>14.06974058040872</v>
+      </c>
+      <c r="L103" s="154">
+        <v>3.1477134558278972</v>
+      </c>
+      <c r="M103" s="154">
+        <v>19.86775276673232</v>
+      </c>
+      <c r="N103" s="154">
+        <v>1.228861261493746</v>
+      </c>
+      <c r="O103" s="155">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="169" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="106" spans="1:15" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="166" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="167" t="s">
+        <v>42</v>
+      </c>
+      <c r="C106" s="167" t="s">
+        <v>43</v>
+      </c>
+      <c r="D106" s="167" t="s">
+        <v>44</v>
+      </c>
+      <c r="E106" s="167" t="s">
+        <v>47</v>
+      </c>
+      <c r="F106" s="167" t="s">
+        <v>46</v>
+      </c>
+      <c r="G106" s="168" t="s">
+        <v>45</v>
+      </c>
+      <c r="H106" s="163"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A107" s="151">
+        <v>2.8</v>
+      </c>
+      <c r="B107" s="150">
+        <v>0.47</v>
+      </c>
+      <c r="C107" s="150">
+        <v>14.8</v>
+      </c>
+      <c r="D107" s="150">
+        <v>28</v>
+      </c>
+      <c r="E107" s="150">
+        <v>51</v>
+      </c>
+      <c r="F107" s="150">
+        <v>49</v>
+      </c>
+      <c r="G107" s="152">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A108" s="151">
+        <v>1.5</v>
+      </c>
+      <c r="B108" s="150">
+        <v>0.22</v>
+      </c>
+      <c r="C108" s="150">
+        <v>15.7</v>
+      </c>
+      <c r="D108" s="150">
+        <v>27</v>
+      </c>
+      <c r="E108" s="150">
+        <v>51</v>
+      </c>
+      <c r="F108" s="150">
+        <v>49</v>
+      </c>
+      <c r="G108" s="152">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A109" s="151">
+        <v>16.8</v>
+      </c>
+      <c r="B109" s="150">
+        <v>1.23</v>
+      </c>
+      <c r="C109" s="150">
+        <v>12.4</v>
+      </c>
+      <c r="D109" s="150">
+        <v>29</v>
+      </c>
+      <c r="E109" s="150">
+        <v>51</v>
+      </c>
+      <c r="F109" s="150">
+        <v>49</v>
+      </c>
+      <c r="G109" s="152">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A110" s="151">
+        <v>1.2</v>
+      </c>
+      <c r="B110" s="150">
+        <v>0.08</v>
+      </c>
+      <c r="C110" s="150">
+        <v>14</v>
+      </c>
+      <c r="D110" s="150">
+        <v>27</v>
+      </c>
+      <c r="E110" s="150">
+        <v>50</v>
+      </c>
+      <c r="F110" s="150">
+        <v>50</v>
+      </c>
+      <c r="G110" s="152">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A111" s="151">
+        <v>22.4</v>
+      </c>
+      <c r="B111" s="150">
+        <v>2.23</v>
+      </c>
+      <c r="C111" s="150">
+        <v>13.8</v>
+      </c>
+      <c r="D111" s="150">
+        <v>30</v>
+      </c>
+      <c r="E111" s="150">
+        <v>52</v>
+      </c>
+      <c r="F111" s="150">
+        <v>48</v>
+      </c>
+      <c r="G111" s="152">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="153">
+        <v>3.5</v>
+      </c>
+      <c r="B112" s="154">
+        <v>0.5</v>
+      </c>
+      <c r="C112" s="154">
+        <v>13</v>
+      </c>
+      <c r="D112" s="154">
+        <v>30</v>
+      </c>
+      <c r="E112" s="154">
+        <v>51</v>
+      </c>
+      <c r="F112" s="154">
+        <v>49</v>
+      </c>
+      <c r="G112" s="155">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="141" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="142" t="s">
+        <v>34</v>
+      </c>
+      <c r="B120" s="143">
+        <v>7.3</v>
+      </c>
+      <c r="C120" s="144">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D120" s="143">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E120" s="143">
+        <v>33</v>
+      </c>
+      <c r="F120" s="143">
+        <v>52</v>
+      </c>
+      <c r="G120" s="143">
+        <v>48</v>
+      </c>
+      <c r="H120" s="145">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B121" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C121" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="D121" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="E121" s="1">
+        <v>28</v>
+      </c>
+      <c r="F121" s="1">
+        <v>51</v>
+      </c>
+      <c r="G121" s="1">
+        <v>49</v>
+      </c>
+      <c r="H121" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="C122" s="8">
+        <v>0.53</v>
+      </c>
+      <c r="D122" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="E122" s="1">
+        <v>31</v>
+      </c>
+      <c r="F122" s="1">
+        <v>52</v>
+      </c>
+      <c r="G122" s="1">
+        <v>48</v>
+      </c>
+      <c r="H122" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C123" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D123" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="E123" s="1">
+        <v>29</v>
+      </c>
+      <c r="F123" s="1">
+        <v>51</v>
+      </c>
+      <c r="G123" s="1">
+        <v>49</v>
+      </c>
+      <c r="H123" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B124" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C124" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D124" s="1">
+        <v>22</v>
+      </c>
+      <c r="E124" s="1">
+        <v>24</v>
+      </c>
+      <c r="F124" s="1">
+        <v>50</v>
+      </c>
+      <c r="G124" s="1">
+        <v>50</v>
+      </c>
+      <c r="H124" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="149" t="s">
+        <v>28</v>
+      </c>
+      <c r="B125" s="146">
+        <v>0.8</v>
+      </c>
+      <c r="C125" s="147">
+        <v>0.04</v>
+      </c>
+      <c r="D125" s="146">
+        <v>15</v>
+      </c>
+      <c r="E125" s="146">
+        <v>28</v>
+      </c>
+      <c r="F125" s="146">
+        <v>52</v>
+      </c>
+      <c r="G125" s="146">
+        <v>48</v>
+      </c>
+      <c r="H125" s="148">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="58">
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="A77:H78"/>
     <mergeCell ref="L61:S61"/>
     <mergeCell ref="L62:S72"/>
     <mergeCell ref="I41:I42"/>
@@ -9480,7 +11155,6 @@
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G47:H47"/>
     <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G7:G8"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="E41:E42"/>
@@ -9501,8 +11175,11 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>